<commit_message>
Fixing the buttons functionalities.
</commit_message>
<xml_diff>
--- a/files/sales.xlsx
+++ b/files/sales.xlsx
@@ -9,9 +9,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>test product</t>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test 3</t>
   </si>
 </sst>
 </file>
@@ -61,24 +64,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
     <col min="4" max="4" width="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>123654</v>
+        <v>123456</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1"/>
+      <c r="C1">
+        <v>130</v>
+      </c>
       <c r="D1">
-        <v>4</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>123654</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>260</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>